<commit_message>
Rename project to parkradar
</commit_message>
<xml_diff>
--- a/ml-development/data/Dataset simplified.xlsx
+++ b/ml-development/data/Dataset simplified.xlsx
@@ -5,16 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pookhaosc/Workspace/ATLAS/Semester 4/Project/parking-app/ml-development/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pookhaosc/Workspace/ATLAS/Semester 4/Project/ezpark/ml-development/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A14650E-BE89-C94C-B0B6-D9997B603AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A040B12F-13D0-084D-844C-5504EBE2B29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Dataset!$C$2:$C$241</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Dataset!$D$2:$D$241</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Dataset!$C$2:$C$241</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Dataset!$D$2:$D$241</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -54,7 +60,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="172" formatCode="h:mm:ss;@"/>
+    <numFmt numFmtId="164" formatCode="h:mm:ss;@"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -535,7 +541,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -593,6 +599,2297 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="nl-NL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Dataset!$C$2:$C$241</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="240"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.89999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.7999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.1000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>5.7</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>5.9</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>6.1</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>6.2000000000000011</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>6.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>6.7</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>6.8</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>6.9</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>7.1</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>7.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>7.2999999999999989</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>7.7000000000000011</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>7.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>7.9</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>8.1</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>8.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>8.4</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>8.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>8.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>8.9</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>9.1</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>9.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>9.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>9.6</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>9.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>9.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>9.9</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>10.1</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>10.199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>10.3</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>10.4</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>10.6</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>10.7</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>10.8</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>10.9</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>11.1</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>11.2</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>11.3</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>11.4</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>11.6</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>11.7</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>11.8</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>11.9</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>12.1</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>12.2</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>12.3</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>12.400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>12.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>12.7</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>12.8</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>12.899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>13.099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>13.2</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>13.3</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>13.4</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>13.6</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>13.7</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>13.8</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>13.900000000000002</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>14.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>14.2</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>14.3</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>14.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>14.599999999999998</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>14.7</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>14.8</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>14.9</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>15.1</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>15.2</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>15.3</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>15.400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>15.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>15.8</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>15.899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>16.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>16.2</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>16.3</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>16.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>16.5</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>16.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>16.7</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>16.8</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>16.899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>17.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>17.2</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>17.3</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>17.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>17.5</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>17.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>17.7</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>17.8</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>17.899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>18.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>18.2</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>18.3</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>18.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>18.5</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>18.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>18.7</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>18.8</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>18.899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>19.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>19.2</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>19.3</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>19.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>19.5</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>19.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>19.7</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>19.8</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>19.899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>20.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>20.2</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>20.3</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>20.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>20.5</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>20.6</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>20.7</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>20.8</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>20.9</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>21.1</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>21.2</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>21.3</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>21.4</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>21.6</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>21.7</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>21.8</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>21.9</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>22.1</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>22.2</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>22.3</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>22.4</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>22.5</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>22.6</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>22.7</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>22.8</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>22.9</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>23.1</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>23.2</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>23.3</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>23.4</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>23.5</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>23.6</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>23.7</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>23.8</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>23.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Dataset!$D$2:$D$241</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="240"/>
+                <c:pt idx="0">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.17</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>0.17</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>0.37</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>0.37</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>0.37</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>0.37</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>0.37</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>0.41</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>0.51</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>0.51</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>0.51</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>0.84</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-00DD-C844-AF78-8AA480E751D7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1948057232"/>
+        <c:axId val="1948058880"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1948057232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1948058880"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1948058880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1948057232"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nl-NL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>275055</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>155631</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>332205</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>111181</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Grafiek 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50388D39-FC17-9ADB-AC77-1C584E6CACA0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -894,8 +3191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E5008"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="120" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="100" zoomScaleSheetLayoutView="120" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -91053,5 +93350,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>